<commit_message>
latex code for tables
</commit_message>
<xml_diff>
--- a/HMresults.xlsx
+++ b/HMresults.xlsx
@@ -509,7 +509,7 @@
         <v>9305.011780647301</v>
       </c>
       <c r="G2" t="n">
-        <v>4522.999898765502</v>
+        <v>4445.37816546568</v>
       </c>
       <c r="H2" t="n">
         <v>9305.094045834723</v>
@@ -545,7 +545,7 @@
         <v>7160.731393697739</v>
       </c>
       <c r="G3" t="n">
-        <v>3575.438939696558</v>
+        <v>3522.860453977319</v>
       </c>
       <c r="H3" t="n">
         <v>7161.550341752863</v>
@@ -581,7 +581,7 @@
         <v>9808.895882357603</v>
       </c>
       <c r="G4" t="n">
-        <v>7093.196533119267</v>
+        <v>6675.338893189715</v>
       </c>
       <c r="H4" t="n">
         <v>9808.183334351626</v>
@@ -617,7 +617,7 @@
         <v>7546.419931889002</v>
       </c>
       <c r="G5" t="n">
-        <v>3586.827338855677</v>
+        <v>3586.112347731234</v>
       </c>
       <c r="H5" t="n">
         <v>7547.239493817145</v>
@@ -653,7 +653,7 @@
         <v>0.891639435017483</v>
       </c>
       <c r="G6" t="n">
-        <v>0.760465487061352</v>
+        <v>0.756964996274725</v>
       </c>
       <c r="H6" t="n">
         <v>0.8895213759393502</v>
@@ -689,7 +689,7 @@
         <v>0.9777163547046319</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8463514749013837</v>
+        <v>0.8419859648424165</v>
       </c>
       <c r="H7" t="n">
         <v>0.9789210989022098</v>
@@ -725,7 +725,7 @@
         <v>0.9454546022977456</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8466630735609638</v>
+        <v>0.8323486429190367</v>
       </c>
       <c r="H8" t="n">
         <v>0.9453051029920841</v>
@@ -761,7 +761,7 @@
         <v>0.9537139738668391</v>
       </c>
       <c r="G9" t="n">
-        <v>0.681920460291361</v>
+        <v>0.6867279060865942</v>
       </c>
       <c r="H9" t="n">
         <v>0.9499240715175293</v>
@@ -797,7 +797,7 @@
         <v>0.3823211453519559</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3627535670531983</v>
+        <v>0.3639975625079706</v>
       </c>
       <c r="H10" t="n">
         <v>0.3828492042521351</v>
@@ -833,7 +833,7 @@
         <v>0.3421680728308225</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3922763516829432</v>
+        <v>0.3944289289741915</v>
       </c>
       <c r="H11" t="n">
         <v>0.3416898588512407</v>
@@ -869,7 +869,7 @@
         <v>0.3547025765341768</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3272494235448429</v>
+        <v>0.3200883900502076</v>
       </c>
       <c r="H12" t="n">
         <v>0.3544454055087202</v>
@@ -905,7 +905,7 @@
         <v>0.3604341704326903</v>
       </c>
       <c r="G13" t="n">
-        <v>0.446144623607641</v>
+        <v>0.4438841847577117</v>
       </c>
       <c r="H13" t="n">
         <v>0.3619390878530176</v>

</xml_diff>